<commit_message>
Added numeric comparison for keys while sorting a table and cleaned mouse handling of Pokimon
</commit_message>
<xml_diff>
--- a/GameBasic/db_tables/pokimonMoves.xlsx
+++ b/GameBasic/db_tables/pokimonMoves.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
   <si>
     <t>Time</t>
   </si>
@@ -26,10 +26,10 @@
     <t>Direction</t>
   </si>
   <si>
-    <t>10200</t>
-  </si>
-  <si>
-    <t>440</t>
+    <t>300</t>
+  </si>
+  <si>
+    <t>110</t>
   </si>
   <si>
     <t>100</t>
@@ -38,34 +38,16 @@
     <t>RIGHT</t>
   </si>
   <si>
-    <t>10500</t>
-  </si>
-  <si>
-    <t>450</t>
-  </si>
-  <si>
-    <t>10800</t>
-  </si>
-  <si>
-    <t>460</t>
-  </si>
-  <si>
-    <t>11100</t>
-  </si>
-  <si>
-    <t>470</t>
-  </si>
-  <si>
-    <t>11400</t>
-  </si>
-  <si>
-    <t>480</t>
-  </si>
-  <si>
-    <t>11700</t>
-  </si>
-  <si>
-    <t>490</t>
+    <t>600</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>900</t>
+  </si>
+  <si>
+    <t>130</t>
   </si>
   <si>
     <t>1200</t>
@@ -74,12 +56,6 @@
     <t>140</t>
   </si>
   <si>
-    <t>12000</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
     <t>1500</t>
   </si>
   <si>
@@ -110,12 +86,6 @@
     <t>190</t>
   </si>
   <si>
-    <t>300</t>
-  </si>
-  <si>
-    <t>110</t>
-  </si>
-  <si>
     <t>3000</t>
   </si>
   <si>
@@ -176,12 +146,6 @@
     <t>290</t>
   </si>
   <si>
-    <t>600</t>
-  </si>
-  <si>
-    <t>120</t>
-  </si>
-  <si>
     <t>6000</t>
   </si>
   <si>
@@ -225,48 +189,6 @@
   </si>
   <si>
     <t>370</t>
-  </si>
-  <si>
-    <t>8400</t>
-  </si>
-  <si>
-    <t>380</t>
-  </si>
-  <si>
-    <t>8700</t>
-  </si>
-  <si>
-    <t>390</t>
-  </si>
-  <si>
-    <t>900</t>
-  </si>
-  <si>
-    <t>130</t>
-  </si>
-  <si>
-    <t>9000</t>
-  </si>
-  <si>
-    <t>400</t>
-  </si>
-  <si>
-    <t>9300</t>
-  </si>
-  <si>
-    <t>410</t>
-  </si>
-  <si>
-    <t>9600</t>
-  </si>
-  <si>
-    <t>420</t>
-  </si>
-  <si>
-    <t>9900</t>
-  </si>
-  <si>
-    <t>430</t>
   </si>
 </sst>
 </file>
@@ -311,7 +233,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -602,7 +524,7 @@
         <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="C21" t="s">
         <v>6</v>
@@ -613,10 +535,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
         <v>46</v>
-      </c>
-      <c r="B22" t="s">
-        <v>47</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
@@ -627,10 +549,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" t="s">
         <v>48</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
       </c>
       <c r="C23" t="s">
         <v>6</v>
@@ -641,10 +563,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
         <v>50</v>
-      </c>
-      <c r="B24" t="s">
-        <v>51</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
@@ -655,10 +577,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" t="s">
         <v>52</v>
-      </c>
-      <c r="B25" t="s">
-        <v>53</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
@@ -669,10 +591,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" t="s">
         <v>54</v>
-      </c>
-      <c r="B26" t="s">
-        <v>55</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
@@ -683,10 +605,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" t="s">
         <v>56</v>
-      </c>
-      <c r="B27" t="s">
-        <v>32</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
@@ -706,188 +628,6 @@
         <v>6</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
-        <v>65</v>
-      </c>
-      <c r="B32" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
-        <v>69</v>
-      </c>
-      <c r="B34" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" t="s">
-        <v>74</v>
-      </c>
-      <c r="C36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D36" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s">
-        <v>75</v>
-      </c>
-      <c r="B37" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D37" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s">
-        <v>77</v>
-      </c>
-      <c r="B38" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s">
-        <v>79</v>
-      </c>
-      <c r="B39" t="s">
-        <v>80</v>
-      </c>
-      <c r="C39" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s">
-        <v>81</v>
-      </c>
-      <c r="B40" t="s">
-        <v>82</v>
-      </c>
-      <c r="C40" t="s">
-        <v>6</v>
-      </c>
-      <c r="D40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s">
-        <v>83</v>
-      </c>
-      <c r="B41" t="s">
-        <v>84</v>
-      </c>
-      <c r="C41" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ExcelTable was modified so that the row of fields (values) includes the key as well to allow uniform handling of the values.
</commit_message>
<xml_diff>
--- a/GameBasic/db_tables/pokimonMoves.xlsx
+++ b/GameBasic/db_tables/pokimonMoves.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="174">
   <si>
     <t>Time</t>
   </si>
@@ -189,6 +189,351 @@
   </si>
   <si>
     <t>370</t>
+  </si>
+  <si>
+    <t>8400</t>
+  </si>
+  <si>
+    <t>380</t>
+  </si>
+  <si>
+    <t>8700</t>
+  </si>
+  <si>
+    <t>390</t>
+  </si>
+  <si>
+    <t>9000</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>9300</t>
+  </si>
+  <si>
+    <t>410</t>
+  </si>
+  <si>
+    <t>9600</t>
+  </si>
+  <si>
+    <t>420</t>
+  </si>
+  <si>
+    <t>9900</t>
+  </si>
+  <si>
+    <t>430</t>
+  </si>
+  <si>
+    <t>10200</t>
+  </si>
+  <si>
+    <t>440</t>
+  </si>
+  <si>
+    <t>10500</t>
+  </si>
+  <si>
+    <t>450</t>
+  </si>
+  <si>
+    <t>10800</t>
+  </si>
+  <si>
+    <t>460</t>
+  </si>
+  <si>
+    <t>11100</t>
+  </si>
+  <si>
+    <t>470</t>
+  </si>
+  <si>
+    <t>11400</t>
+  </si>
+  <si>
+    <t>480</t>
+  </si>
+  <si>
+    <t>11700</t>
+  </si>
+  <si>
+    <t>490</t>
+  </si>
+  <si>
+    <t>12000</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>12300</t>
+  </si>
+  <si>
+    <t>510</t>
+  </si>
+  <si>
+    <t>12600</t>
+  </si>
+  <si>
+    <t>520</t>
+  </si>
+  <si>
+    <t>12900</t>
+  </si>
+  <si>
+    <t>530</t>
+  </si>
+  <si>
+    <t>13200</t>
+  </si>
+  <si>
+    <t>540</t>
+  </si>
+  <si>
+    <t>13500</t>
+  </si>
+  <si>
+    <t>550</t>
+  </si>
+  <si>
+    <t>13800</t>
+  </si>
+  <si>
+    <t>560</t>
+  </si>
+  <si>
+    <t>14100</t>
+  </si>
+  <si>
+    <t>570</t>
+  </si>
+  <si>
+    <t>14400</t>
+  </si>
+  <si>
+    <t>580</t>
+  </si>
+  <si>
+    <t>14700</t>
+  </si>
+  <si>
+    <t>590</t>
+  </si>
+  <si>
+    <t>15000</t>
+  </si>
+  <si>
+    <t>15300</t>
+  </si>
+  <si>
+    <t>610</t>
+  </si>
+  <si>
+    <t>15600</t>
+  </si>
+  <si>
+    <t>620</t>
+  </si>
+  <si>
+    <t>15900</t>
+  </si>
+  <si>
+    <t>630</t>
+  </si>
+  <si>
+    <t>16200</t>
+  </si>
+  <si>
+    <t>640</t>
+  </si>
+  <si>
+    <t>16500</t>
+  </si>
+  <si>
+    <t>650</t>
+  </si>
+  <si>
+    <t>16800</t>
+  </si>
+  <si>
+    <t>660</t>
+  </si>
+  <si>
+    <t>17100</t>
+  </si>
+  <si>
+    <t>670</t>
+  </si>
+  <si>
+    <t>17400</t>
+  </si>
+  <si>
+    <t>680</t>
+  </si>
+  <si>
+    <t>17700</t>
+  </si>
+  <si>
+    <t>690</t>
+  </si>
+  <si>
+    <t>23100</t>
+  </si>
+  <si>
+    <t>LEFT</t>
+  </si>
+  <si>
+    <t>23400</t>
+  </si>
+  <si>
+    <t>23700</t>
+  </si>
+  <si>
+    <t>24000</t>
+  </si>
+  <si>
+    <t>24300</t>
+  </si>
+  <si>
+    <t>24600</t>
+  </si>
+  <si>
+    <t>24900</t>
+  </si>
+  <si>
+    <t>25200</t>
+  </si>
+  <si>
+    <t>25500</t>
+  </si>
+  <si>
+    <t>25800</t>
+  </si>
+  <si>
+    <t>26100</t>
+  </si>
+  <si>
+    <t>26400</t>
+  </si>
+  <si>
+    <t>26700</t>
+  </si>
+  <si>
+    <t>DOWN</t>
+  </si>
+  <si>
+    <t>27000</t>
+  </si>
+  <si>
+    <t>27300</t>
+  </si>
+  <si>
+    <t>27600</t>
+  </si>
+  <si>
+    <t>27900</t>
+  </si>
+  <si>
+    <t>28200</t>
+  </si>
+  <si>
+    <t>28500</t>
+  </si>
+  <si>
+    <t>28800</t>
+  </si>
+  <si>
+    <t>29100</t>
+  </si>
+  <si>
+    <t>29400</t>
+  </si>
+  <si>
+    <t>29700</t>
+  </si>
+  <si>
+    <t>30000</t>
+  </si>
+  <si>
+    <t>30300</t>
+  </si>
+  <si>
+    <t>30600</t>
+  </si>
+  <si>
+    <t>30900</t>
+  </si>
+  <si>
+    <t>31200</t>
+  </si>
+  <si>
+    <t>31500</t>
+  </si>
+  <si>
+    <t>31800</t>
+  </si>
+  <si>
+    <t>32100</t>
+  </si>
+  <si>
+    <t>32400</t>
+  </si>
+  <si>
+    <t>32700</t>
+  </si>
+  <si>
+    <t>33000</t>
+  </si>
+  <si>
+    <t>33300</t>
+  </si>
+  <si>
+    <t>33600</t>
+  </si>
+  <si>
+    <t>33900</t>
+  </si>
+  <si>
+    <t>34200</t>
+  </si>
+  <si>
+    <t>34500</t>
+  </si>
+  <si>
+    <t>34800</t>
+  </si>
+  <si>
+    <t>35100</t>
+  </si>
+  <si>
+    <t>35400</t>
+  </si>
+  <si>
+    <t>35700</t>
+  </si>
+  <si>
+    <t>36000</t>
+  </si>
+  <si>
+    <t>36300</t>
+  </si>
+  <si>
+    <t>36600</t>
+  </si>
+  <si>
+    <t>36900</t>
+  </si>
+  <si>
+    <t>37200</t>
+  </si>
+  <si>
+    <t>37500</t>
+  </si>
+  <si>
+    <t>37800</t>
   </si>
 </sst>
 </file>
@@ -233,7 +578,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D110"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -631,6 +976,1154 @@
         <v>7</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>67</v>
+      </c>
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>91</v>
+      </c>
+      <c r="B45" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>93</v>
+      </c>
+      <c r="B46" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" t="s">
+        <v>100</v>
+      </c>
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>103</v>
+      </c>
+      <c r="B51" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>104</v>
+      </c>
+      <c r="B52" t="s">
+        <v>105</v>
+      </c>
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>106</v>
+      </c>
+      <c r="B53" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>108</v>
+      </c>
+      <c r="B54" t="s">
+        <v>109</v>
+      </c>
+      <c r="C54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>110</v>
+      </c>
+      <c r="B55" t="s">
+        <v>111</v>
+      </c>
+      <c r="C55" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>112</v>
+      </c>
+      <c r="B56" t="s">
+        <v>113</v>
+      </c>
+      <c r="C56" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>114</v>
+      </c>
+      <c r="B57" t="s">
+        <v>115</v>
+      </c>
+      <c r="C57" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" t="s">
+        <v>117</v>
+      </c>
+      <c r="C58" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59" t="s">
+        <v>119</v>
+      </c>
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>120</v>
+      </c>
+      <c r="B60" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>122</v>
+      </c>
+      <c r="B61" t="s">
+        <v>119</v>
+      </c>
+      <c r="C61" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>124</v>
+      </c>
+      <c r="B62" t="s">
+        <v>117</v>
+      </c>
+      <c r="C62" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>125</v>
+      </c>
+      <c r="B63" t="s">
+        <v>115</v>
+      </c>
+      <c r="C63" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" t="s">
+        <v>113</v>
+      </c>
+      <c r="C64" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>127</v>
+      </c>
+      <c r="B65" t="s">
+        <v>111</v>
+      </c>
+      <c r="C65" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>128</v>
+      </c>
+      <c r="B66" t="s">
+        <v>109</v>
+      </c>
+      <c r="C66" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>129</v>
+      </c>
+      <c r="B67" t="s">
+        <v>107</v>
+      </c>
+      <c r="C67" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>130</v>
+      </c>
+      <c r="B68" t="s">
+        <v>105</v>
+      </c>
+      <c r="C68" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>131</v>
+      </c>
+      <c r="B69" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>132</v>
+      </c>
+      <c r="B70" t="s">
+        <v>102</v>
+      </c>
+      <c r="C70" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>133</v>
+      </c>
+      <c r="B71" t="s">
+        <v>100</v>
+      </c>
+      <c r="C71" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>134</v>
+      </c>
+      <c r="B72" t="s">
+        <v>98</v>
+      </c>
+      <c r="C72" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>135</v>
+      </c>
+      <c r="B73" t="s">
+        <v>98</v>
+      </c>
+      <c r="C73" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>137</v>
+      </c>
+      <c r="B74" t="s">
+        <v>98</v>
+      </c>
+      <c r="C74" t="s">
+        <v>9</v>
+      </c>
+      <c r="D74" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>138</v>
+      </c>
+      <c r="B75" t="s">
+        <v>98</v>
+      </c>
+      <c r="C75" t="s">
+        <v>11</v>
+      </c>
+      <c r="D75" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>139</v>
+      </c>
+      <c r="B76" t="s">
+        <v>98</v>
+      </c>
+      <c r="C76" t="s">
+        <v>13</v>
+      </c>
+      <c r="D76" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>140</v>
+      </c>
+      <c r="B77" t="s">
+        <v>96</v>
+      </c>
+      <c r="C77" t="s">
+        <v>13</v>
+      </c>
+      <c r="D77" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>141</v>
+      </c>
+      <c r="B78" t="s">
+        <v>94</v>
+      </c>
+      <c r="C78" t="s">
+        <v>13</v>
+      </c>
+      <c r="D78" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>142</v>
+      </c>
+      <c r="B79" t="s">
+        <v>94</v>
+      </c>
+      <c r="C79" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>143</v>
+      </c>
+      <c r="B80" t="s">
+        <v>94</v>
+      </c>
+      <c r="C80" t="s">
+        <v>17</v>
+      </c>
+      <c r="D80" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>144</v>
+      </c>
+      <c r="B81" t="s">
+        <v>92</v>
+      </c>
+      <c r="C81" t="s">
+        <v>17</v>
+      </c>
+      <c r="D81" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>145</v>
+      </c>
+      <c r="B82" t="s">
+        <v>90</v>
+      </c>
+      <c r="C82" t="s">
+        <v>17</v>
+      </c>
+      <c r="D82" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>146</v>
+      </c>
+      <c r="B83" t="s">
+        <v>90</v>
+      </c>
+      <c r="C83" t="s">
+        <v>19</v>
+      </c>
+      <c r="D83" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>147</v>
+      </c>
+      <c r="B84" t="s">
+        <v>88</v>
+      </c>
+      <c r="C84" t="s">
+        <v>19</v>
+      </c>
+      <c r="D84" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>148</v>
+      </c>
+      <c r="B85" t="s">
+        <v>86</v>
+      </c>
+      <c r="C85" t="s">
+        <v>19</v>
+      </c>
+      <c r="D85" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>149</v>
+      </c>
+      <c r="B86" t="s">
+        <v>84</v>
+      </c>
+      <c r="C86" t="s">
+        <v>19</v>
+      </c>
+      <c r="D86" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>150</v>
+      </c>
+      <c r="B87" t="s">
+        <v>84</v>
+      </c>
+      <c r="C87" t="s">
+        <v>21</v>
+      </c>
+      <c r="D87" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
+        <v>151</v>
+      </c>
+      <c r="B88" t="s">
+        <v>84</v>
+      </c>
+      <c r="C88" t="s">
+        <v>23</v>
+      </c>
+      <c r="D88" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>152</v>
+      </c>
+      <c r="B89" t="s">
+        <v>82</v>
+      </c>
+      <c r="C89" t="s">
+        <v>23</v>
+      </c>
+      <c r="D89" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>153</v>
+      </c>
+      <c r="B90" t="s">
+        <v>80</v>
+      </c>
+      <c r="C90" t="s">
+        <v>23</v>
+      </c>
+      <c r="D90" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>154</v>
+      </c>
+      <c r="B91" t="s">
+        <v>78</v>
+      </c>
+      <c r="C91" t="s">
+        <v>23</v>
+      </c>
+      <c r="D91" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>155</v>
+      </c>
+      <c r="B92" t="s">
+        <v>78</v>
+      </c>
+      <c r="C92" t="s">
+        <v>25</v>
+      </c>
+      <c r="D92" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>156</v>
+      </c>
+      <c r="B93" t="s">
+        <v>78</v>
+      </c>
+      <c r="C93" t="s">
+        <v>27</v>
+      </c>
+      <c r="D93" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>157</v>
+      </c>
+      <c r="B94" t="s">
+        <v>78</v>
+      </c>
+      <c r="C94" t="s">
+        <v>29</v>
+      </c>
+      <c r="D94" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>158</v>
+      </c>
+      <c r="B95" t="s">
+        <v>76</v>
+      </c>
+      <c r="C95" t="s">
+        <v>29</v>
+      </c>
+      <c r="D95" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>159</v>
+      </c>
+      <c r="B96" t="s">
+        <v>74</v>
+      </c>
+      <c r="C96" t="s">
+        <v>29</v>
+      </c>
+      <c r="D96" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>160</v>
+      </c>
+      <c r="B97" t="s">
+        <v>72</v>
+      </c>
+      <c r="C97" t="s">
+        <v>29</v>
+      </c>
+      <c r="D97" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>161</v>
+      </c>
+      <c r="B98" t="s">
+        <v>70</v>
+      </c>
+      <c r="C98" t="s">
+        <v>29</v>
+      </c>
+      <c r="D98" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>162</v>
+      </c>
+      <c r="B99" t="s">
+        <v>68</v>
+      </c>
+      <c r="C99" t="s">
+        <v>29</v>
+      </c>
+      <c r="D99" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>163</v>
+      </c>
+      <c r="B100" t="s">
+        <v>66</v>
+      </c>
+      <c r="C100" t="s">
+        <v>29</v>
+      </c>
+      <c r="D100" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>164</v>
+      </c>
+      <c r="B101" t="s">
+        <v>64</v>
+      </c>
+      <c r="C101" t="s">
+        <v>29</v>
+      </c>
+      <c r="D101" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>165</v>
+      </c>
+      <c r="B102" t="s">
+        <v>62</v>
+      </c>
+      <c r="C102" t="s">
+        <v>29</v>
+      </c>
+      <c r="D102" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>166</v>
+      </c>
+      <c r="B103" t="s">
+        <v>60</v>
+      </c>
+      <c r="C103" t="s">
+        <v>29</v>
+      </c>
+      <c r="D103" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>167</v>
+      </c>
+      <c r="B104" t="s">
+        <v>58</v>
+      </c>
+      <c r="C104" t="s">
+        <v>29</v>
+      </c>
+      <c r="D104" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>168</v>
+      </c>
+      <c r="B105" t="s">
+        <v>56</v>
+      </c>
+      <c r="C105" t="s">
+        <v>29</v>
+      </c>
+      <c r="D105" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>169</v>
+      </c>
+      <c r="B106" t="s">
+        <v>54</v>
+      </c>
+      <c r="C106" t="s">
+        <v>29</v>
+      </c>
+      <c r="D106" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>170</v>
+      </c>
+      <c r="B107" t="s">
+        <v>52</v>
+      </c>
+      <c r="C107" t="s">
+        <v>29</v>
+      </c>
+      <c r="D107" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>171</v>
+      </c>
+      <c r="B108" t="s">
+        <v>50</v>
+      </c>
+      <c r="C108" t="s">
+        <v>29</v>
+      </c>
+      <c r="D108" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>172</v>
+      </c>
+      <c r="B109" t="s">
+        <v>48</v>
+      </c>
+      <c r="C109" t="s">
+        <v>29</v>
+      </c>
+      <c r="D109" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>173</v>
+      </c>
+      <c r="B110" t="s">
+        <v>46</v>
+      </c>
+      <c r="C110" t="s">
+        <v>29</v>
+      </c>
+      <c r="D110" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Add show table, get input and shape button
</commit_message>
<xml_diff>
--- a/GameBasic/db_tables/pokimonMoves.xlsx
+++ b/GameBasic/db_tables/pokimonMoves.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="41">
   <si>
     <t>Time</t>
   </si>
@@ -26,55 +26,115 @@
     <t>Direction</t>
   </si>
   <si>
+    <t>7200</t>
+  </si>
+  <si>
+    <t>340</t>
+  </si>
+  <si>
+    <t>300</t>
+  </si>
+  <si>
+    <t>LEFT</t>
+  </si>
+  <si>
+    <t>5100</t>
+  </si>
+  <si>
+    <t>370</t>
+  </si>
+  <si>
+    <t>RIGHT</t>
+  </si>
+  <si>
+    <t>3000</t>
+  </si>
+  <si>
+    <t>2700</t>
+  </si>
+  <si>
+    <t>310</t>
+  </si>
+  <si>
+    <t>6900</t>
+  </si>
+  <si>
+    <t>350</t>
+  </si>
+  <si>
+    <t>4800</t>
+  </si>
+  <si>
+    <t>360</t>
+  </si>
+  <si>
+    <t>6000</t>
+  </si>
+  <si>
+    <t>380</t>
+  </si>
+  <si>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>3600</t>
+  </si>
+  <si>
+    <t>320</t>
+  </si>
+  <si>
+    <t>600</t>
+  </si>
+  <si>
+    <t>7800</t>
+  </si>
+  <si>
+    <t>5700</t>
+  </si>
+  <si>
+    <t>390</t>
+  </si>
+  <si>
+    <t>5400</t>
+  </si>
+  <si>
+    <t>7500</t>
+  </si>
+  <si>
+    <t>330</t>
+  </si>
+  <si>
+    <t>2400</t>
+  </si>
+  <si>
+    <t>4500</t>
+  </si>
+  <si>
+    <t>6600</t>
+  </si>
+  <si>
+    <t>6300</t>
+  </si>
+  <si>
+    <t>4200</t>
+  </si>
+  <si>
+    <t>2100</t>
+  </si>
+  <si>
     <t>1800</t>
   </si>
   <si>
-    <t>360</t>
-  </si>
-  <si>
-    <t>300</t>
-  </si>
-  <si>
-    <t>RIGHT</t>
-  </si>
-  <si>
-    <t>310</t>
-  </si>
-  <si>
-    <t>1500</t>
-  </si>
-  <si>
-    <t>350</t>
-  </si>
-  <si>
-    <t>2400</t>
-  </si>
-  <si>
-    <t>380</t>
-  </si>
-  <si>
-    <t>600</t>
-  </si>
-  <si>
-    <t>320</t>
-  </si>
-  <si>
     <t>1200</t>
   </si>
   <si>
-    <t>340</t>
-  </si>
-  <si>
-    <t>2100</t>
-  </si>
-  <si>
-    <t>370</t>
+    <t>3300</t>
   </si>
   <si>
     <t>900</t>
   </si>
   <si>
-    <t>330</t>
+    <t>3900</t>
   </si>
 </sst>
 </file>
@@ -119,7 +179,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -155,24 +215,24 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -183,10 +243,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -197,10 +257,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -211,24 +271,24 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -239,16 +299,268 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>7</v>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>